<commit_message>
Cambio en las letras mapas de karnaugh y el circuito proteus
</commit_message>
<xml_diff>
--- a/mapas_de_karnaugh.xlsx
+++ b/mapas_de_karnaugh.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ingenieriausacedu-my.sharepoint.com/personal/3140796531218_ingenieria_usac_edu_gt/Documents/USAC CICLO ESCOLAR/9 PRIMER SEMESTRE 2025/ORGA/LABORATORIO/PRACTICAS/PRACTICA1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoséSandoval\Desktop\P1_ORGA_G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="277" documentId="8_{72BA1235-CCA0-4AA9-902A-B8D436147890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB60EB88-1BAC-40D1-A48B-EB5961819BD7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81BC7BE-B8C5-46E6-8A63-72E9D150C75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0ECEB190-8471-4C0B-8113-5907E8DD918B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0ECEB190-8471-4C0B-8113-5907E8DD918B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
   <si>
     <t>00</t>
   </si>
@@ -104,25 +104,22 @@
     <t>10</t>
   </si>
   <si>
-    <t>PARA LETRA A, F, E</t>
-  </si>
-  <si>
-    <t>PARA LETRA B</t>
-  </si>
-  <si>
-    <t>f2 = x' + y + z</t>
-  </si>
-  <si>
-    <t>f3 = z</t>
-  </si>
-  <si>
-    <t>PARA LETRA C, D</t>
-  </si>
-  <si>
-    <t>PARA G</t>
-  </si>
-  <si>
-    <t>f4 = yz' + x'z'</t>
+    <t>PARA A, B, Y F</t>
+  </si>
+  <si>
+    <t>PARA C Y D</t>
+  </si>
+  <si>
+    <t>PARA E Y G</t>
+  </si>
+  <si>
+    <t>F3 = 1</t>
+  </si>
+  <si>
+    <t>F2 = z</t>
+  </si>
+  <si>
+    <t>F1 = yz' + x'z'</t>
   </si>
 </sst>
 </file>
@@ -145,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,25 +157,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="3" tint="0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,7 +324,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -341,7 +332,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -366,24 +356,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -392,11 +375,9 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,10 +459,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -801,10 +778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC71AE7-27C8-4321-8A12-F43BE1CD410D}">
-  <dimension ref="A1:U78"/>
+  <dimension ref="A1:S78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="T21" sqref="T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -816,7 +793,7 @@
     <col min="6" max="12" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -832,30 +809,30 @@
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="28" t="s">
+      <c r="H1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="28" t="s">
+      <c r="I1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="30" t="s">
+      <c r="L1" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="15"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S1" s="14"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -871,33 +848,33 @@
       <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="24">
-        <v>1</v>
-      </c>
-      <c r="G2" s="26">
-        <v>1</v>
-      </c>
-      <c r="H2" s="28">
-        <v>0</v>
-      </c>
-      <c r="I2" s="28">
-        <v>0</v>
-      </c>
-      <c r="J2" s="24">
-        <v>1</v>
-      </c>
-      <c r="K2" s="24">
-        <v>1</v>
-      </c>
-      <c r="L2" s="30">
+      <c r="F2" s="22">
+        <v>1</v>
+      </c>
+      <c r="G2" s="22">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0</v>
+      </c>
+      <c r="I2" s="15">
+        <v>0</v>
+      </c>
+      <c r="J2" s="21">
+        <v>1</v>
+      </c>
+      <c r="K2" s="22">
+        <v>1</v>
+      </c>
+      <c r="L2" s="21">
         <v>1</v>
       </c>
       <c r="N2" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="15"/>
-    </row>
-    <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S2" s="14"/>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -913,30 +890,30 @@
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="24">
-        <v>1</v>
-      </c>
-      <c r="G3" s="26">
-        <v>1</v>
-      </c>
-      <c r="H3" s="28">
-        <v>1</v>
-      </c>
-      <c r="I3" s="28">
-        <v>1</v>
-      </c>
-      <c r="J3" s="24">
-        <v>1</v>
-      </c>
-      <c r="K3" s="24">
-        <v>1</v>
-      </c>
-      <c r="L3" s="30">
-        <v>0</v>
-      </c>
-      <c r="S3" s="15"/>
-    </row>
-    <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F3" s="22">
+        <v>0</v>
+      </c>
+      <c r="G3" s="22">
+        <v>0</v>
+      </c>
+      <c r="H3" s="15">
+        <v>1</v>
+      </c>
+      <c r="I3" s="15">
+        <v>1</v>
+      </c>
+      <c r="J3" s="21">
+        <v>1</v>
+      </c>
+      <c r="K3" s="22">
+        <v>0</v>
+      </c>
+      <c r="L3" s="21">
+        <v>1</v>
+      </c>
+      <c r="S3" s="14"/>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -952,45 +929,45 @@
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="27" t="s">
+      <c r="G4" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="29" t="s">
+      <c r="H4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="28">
-        <v>0</v>
-      </c>
-      <c r="J4" s="24">
-        <v>1</v>
-      </c>
-      <c r="K4" s="24">
-        <v>1</v>
-      </c>
-      <c r="L4" s="30">
-        <v>1</v>
-      </c>
-      <c r="N4" s="14" t="s">
+      <c r="I4" s="15">
+        <v>0</v>
+      </c>
+      <c r="J4" s="21">
+        <v>1</v>
+      </c>
+      <c r="K4" s="22">
+        <v>1</v>
+      </c>
+      <c r="L4" s="21">
+        <v>1</v>
+      </c>
+      <c r="N4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="7" t="s">
+      <c r="O4" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="R4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="15"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S4" s="14"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1006,45 +983,45 @@
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="24">
-        <v>1</v>
-      </c>
-      <c r="G5" s="26">
-        <v>1</v>
-      </c>
-      <c r="H5" s="28">
-        <v>1</v>
-      </c>
-      <c r="I5" s="28">
-        <v>1</v>
-      </c>
-      <c r="J5" s="24">
-        <v>1</v>
-      </c>
-      <c r="K5" s="24">
-        <v>1</v>
-      </c>
-      <c r="L5" s="30">
-        <v>0</v>
-      </c>
-      <c r="N5" s="13">
-        <v>0</v>
-      </c>
-      <c r="O5" s="20">
-        <v>1</v>
-      </c>
-      <c r="P5" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="17">
-        <v>1</v>
-      </c>
-      <c r="R5" s="17">
-        <v>1</v>
-      </c>
-      <c r="S5" s="15"/>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F5" s="22">
+        <v>0</v>
+      </c>
+      <c r="G5" s="22">
+        <v>0</v>
+      </c>
+      <c r="H5" s="15">
+        <v>1</v>
+      </c>
+      <c r="I5" s="15">
+        <v>1</v>
+      </c>
+      <c r="J5" s="21">
+        <v>1</v>
+      </c>
+      <c r="K5" s="22">
+        <v>0</v>
+      </c>
+      <c r="L5" s="21">
+        <v>1</v>
+      </c>
+      <c r="N5" s="12">
+        <v>0</v>
+      </c>
+      <c r="O5" s="26">
+        <v>1</v>
+      </c>
+      <c r="P5" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>0</v>
+      </c>
+      <c r="R5" s="24">
+        <v>1</v>
+      </c>
+      <c r="S5" s="14"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1060,47 +1037,47 @@
       <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="24">
-        <v>1</v>
-      </c>
-      <c r="G6" s="26">
-        <v>0</v>
-      </c>
-      <c r="H6" s="28">
-        <v>0</v>
-      </c>
-      <c r="I6" s="28">
-        <v>0</v>
-      </c>
-      <c r="J6" s="24">
-        <v>1</v>
-      </c>
-      <c r="K6" s="24">
-        <v>1</v>
-      </c>
-      <c r="L6" s="30">
-        <v>0</v>
-      </c>
-      <c r="N6" s="11">
-        <v>1</v>
-      </c>
-      <c r="O6" s="21">
-        <v>1</v>
-      </c>
-      <c r="P6" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="18">
-        <v>1</v>
-      </c>
-      <c r="R6" s="18">
-        <v>1</v>
-      </c>
-      <c r="S6" s="15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F6" s="22">
+        <v>0</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0</v>
+      </c>
+      <c r="I6" s="15">
+        <v>0</v>
+      </c>
+      <c r="J6" s="21">
+        <v>1</v>
+      </c>
+      <c r="K6" s="22">
+        <v>0</v>
+      </c>
+      <c r="L6" s="21">
+        <v>1</v>
+      </c>
+      <c r="N6" s="10">
+        <v>1</v>
+      </c>
+      <c r="O6" s="19">
+        <v>0</v>
+      </c>
+      <c r="P6" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="20">
+        <v>0</v>
+      </c>
+      <c r="R6" s="25">
+        <v>1</v>
+      </c>
+      <c r="S6" s="14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1116,30 +1093,30 @@
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="24">
-        <v>1</v>
-      </c>
-      <c r="G7" s="26">
-        <v>1</v>
-      </c>
-      <c r="H7" s="28">
-        <v>1</v>
-      </c>
-      <c r="I7" s="28">
-        <v>1</v>
-      </c>
-      <c r="J7" s="24">
-        <v>1</v>
-      </c>
-      <c r="K7" s="24">
-        <v>1</v>
-      </c>
-      <c r="L7" s="30">
-        <v>0</v>
-      </c>
-      <c r="S7" s="15"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F7" s="22">
+        <v>0</v>
+      </c>
+      <c r="G7" s="22">
+        <v>0</v>
+      </c>
+      <c r="H7" s="15">
+        <v>1</v>
+      </c>
+      <c r="I7" s="15">
+        <v>1</v>
+      </c>
+      <c r="J7" s="21">
+        <v>1</v>
+      </c>
+      <c r="K7" s="22">
+        <v>0</v>
+      </c>
+      <c r="L7" s="21">
+        <v>1</v>
+      </c>
+      <c r="S7" s="14"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1155,33 +1132,33 @@
       <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="24">
-        <v>1</v>
-      </c>
-      <c r="G8" s="26">
-        <v>1</v>
-      </c>
-      <c r="H8" s="28">
-        <v>0</v>
-      </c>
-      <c r="I8" s="28">
-        <v>0</v>
-      </c>
-      <c r="J8" s="24">
-        <v>1</v>
-      </c>
-      <c r="K8" s="24">
-        <v>1</v>
-      </c>
-      <c r="L8" s="30">
+      <c r="F8" s="22">
+        <v>1</v>
+      </c>
+      <c r="G8" s="22">
+        <v>1</v>
+      </c>
+      <c r="H8" s="15">
+        <v>0</v>
+      </c>
+      <c r="I8" s="15">
+        <v>0</v>
+      </c>
+      <c r="J8" s="21">
+        <v>1</v>
+      </c>
+      <c r="K8" s="22">
+        <v>1</v>
+      </c>
+      <c r="L8" s="21">
         <v>1</v>
       </c>
       <c r="N8" t="s">
         <v>23</v>
       </c>
-      <c r="S8" s="15"/>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S8" s="14"/>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1197,117 +1174,114 @@
       <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="24">
-        <v>1</v>
-      </c>
-      <c r="G9" s="26">
-        <v>1</v>
-      </c>
-      <c r="H9" s="28">
-        <v>1</v>
-      </c>
-      <c r="I9" s="28">
-        <v>1</v>
-      </c>
-      <c r="J9" s="24">
-        <v>1</v>
-      </c>
-      <c r="K9" s="24">
-        <v>1</v>
-      </c>
-      <c r="L9" s="30">
-        <v>0</v>
-      </c>
-      <c r="S9" s="15"/>
-    </row>
-    <row r="10" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N10" s="14" t="s">
+      <c r="F9" s="22">
+        <v>0</v>
+      </c>
+      <c r="G9" s="22">
+        <v>0</v>
+      </c>
+      <c r="H9" s="15">
+        <v>1</v>
+      </c>
+      <c r="I9" s="15">
+        <v>1</v>
+      </c>
+      <c r="J9" s="21">
+        <v>1</v>
+      </c>
+      <c r="K9" s="22">
+        <v>0</v>
+      </c>
+      <c r="L9" s="21">
+        <v>1</v>
+      </c>
+      <c r="S9" s="14"/>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="O10" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="7" t="s">
+      <c r="O10" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R10" s="8" t="s">
+      <c r="R10" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="S10" s="15"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N11" s="13">
-        <v>0</v>
-      </c>
-      <c r="O11" s="19">
-        <v>1</v>
-      </c>
-      <c r="P11" s="22">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="17">
-        <v>1</v>
-      </c>
-      <c r="R11" s="17">
-        <v>1</v>
-      </c>
-      <c r="S11" s="15" t="s">
+      <c r="S10" s="14"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N11" s="12">
+        <v>0</v>
+      </c>
+      <c r="O11" s="17">
+        <v>0</v>
+      </c>
+      <c r="P11" s="24">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="24">
+        <v>1</v>
+      </c>
+      <c r="R11" s="18">
+        <v>0</v>
+      </c>
+      <c r="S11" s="14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N12" s="10">
+        <v>1</v>
+      </c>
+      <c r="O12" s="19">
+        <v>0</v>
+      </c>
+      <c r="P12" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="25">
+        <v>1</v>
+      </c>
+      <c r="R12" s="20">
+        <v>0</v>
+      </c>
+      <c r="S12" s="14"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S13" s="14"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M12" s="3"/>
-      <c r="N12" s="11">
-        <v>1</v>
-      </c>
-      <c r="O12" s="10">
-        <v>0</v>
-      </c>
-      <c r="P12" s="23">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="18">
-        <v>1</v>
-      </c>
-      <c r="R12" s="18">
-        <v>1</v>
-      </c>
-      <c r="S12" s="16"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="S13" s="15"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N14" t="s">
-        <v>26</v>
-      </c>
-      <c r="S14" s="15"/>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S15" s="15"/>
-    </row>
-    <row r="16" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N16" s="14" t="s">
+      <c r="S14" s="14"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S15" s="14"/>
+    </row>
+    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N16" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="O16" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="7" t="s">
+      <c r="O16" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R16" s="8" t="s">
+      <c r="R16" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="S16" s="15"/>
+      <c r="S16" s="14"/>
     </row>
     <row r="17" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G17" s="1"/>
@@ -1315,376 +1289,321 @@
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
-      <c r="N17" s="13">
-        <v>0</v>
-      </c>
-      <c r="O17" s="9">
-        <v>0</v>
-      </c>
-      <c r="P17" s="17">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="17">
-        <v>1</v>
-      </c>
-      <c r="R17" s="17">
-        <v>0</v>
-      </c>
-      <c r="S17" s="15" t="s">
+      <c r="N17" s="12">
+        <v>0</v>
+      </c>
+      <c r="O17" s="17">
+        <v>1</v>
+      </c>
+      <c r="P17" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="18">
+        <v>1</v>
+      </c>
+      <c r="R17" s="18">
+        <v>1</v>
+      </c>
+      <c r="S17" s="14" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G18" s="1"/>
-      <c r="N18" s="11">
-        <v>1</v>
-      </c>
-      <c r="O18" s="10">
-        <v>0</v>
-      </c>
-      <c r="P18" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="18">
-        <v>1</v>
-      </c>
-      <c r="R18" s="18">
-        <v>0</v>
-      </c>
-      <c r="S18" s="15"/>
+      <c r="N18" s="10">
+        <v>1</v>
+      </c>
+      <c r="O18" s="19">
+        <v>1</v>
+      </c>
+      <c r="P18" s="20">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="20">
+        <v>1</v>
+      </c>
+      <c r="R18" s="20">
+        <v>1</v>
+      </c>
+      <c r="S18" s="14"/>
     </row>
     <row r="19" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G19" s="1"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="15"/>
+      <c r="S19" s="14"/>
     </row>
     <row r="20" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="N20" t="s">
-        <v>27</v>
-      </c>
-      <c r="S20" s="15"/>
-    </row>
-    <row r="21" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S21" s="15"/>
-    </row>
-    <row r="22" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N22" s="14" t="s">
+      <c r="S20" s="14"/>
+    </row>
+    <row r="21" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="14"/>
+    </row>
+    <row r="22" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="14"/>
+    </row>
+    <row r="23" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="S23" s="14"/>
+    </row>
+    <row r="24" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="S24" s="14"/>
+    </row>
+    <row r="25" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S25" s="14"/>
+    </row>
+    <row r="26" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="O22" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="7" t="s">
+      <c r="O26" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P26" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R22" s="8" t="s">
+      <c r="R26" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="S22" s="15"/>
-    </row>
-    <row r="23" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="N23" s="13">
-        <v>0</v>
-      </c>
-      <c r="O23" s="20">
-        <v>1</v>
-      </c>
-      <c r="P23" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="6">
-        <v>0</v>
-      </c>
-      <c r="R23" s="31">
-        <v>1</v>
-      </c>
-      <c r="S23" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N24" s="11">
-        <v>1</v>
-      </c>
-      <c r="O24" s="10">
-        <v>0</v>
-      </c>
-      <c r="P24" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="5">
-        <v>0</v>
-      </c>
-      <c r="R24" s="32">
-        <v>1</v>
-      </c>
-      <c r="S24" s="15"/>
-    </row>
-    <row r="25" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="S25" s="15"/>
-    </row>
-    <row r="26" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
-      <c r="S26" s="15"/>
+      <c r="S26" s="14"/>
     </row>
     <row r="27" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="15"/>
-    </row>
-    <row r="28" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="S28" s="15"/>
+      <c r="N27" s="12">
+        <v>0</v>
+      </c>
+      <c r="O27" s="8"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="14"/>
+    </row>
+    <row r="28" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N28" s="10">
+        <v>1</v>
+      </c>
+      <c r="O28" s="9"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="14"/>
     </row>
     <row r="29" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="S29" s="15"/>
-    </row>
-    <row r="30" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S30" s="15"/>
+      <c r="S29" s="14"/>
+    </row>
+    <row r="30" spans="7:19" x14ac:dyDescent="0.25">
+      <c r="S30" s="14"/>
     </row>
     <row r="31" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N31" s="14" t="s">
+      <c r="S31" s="14"/>
+    </row>
+    <row r="32" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N32" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="O31" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P31" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="7" t="s">
+      <c r="O32" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P32" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R31" s="8" t="s">
+      <c r="R32" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="S31" s="15"/>
-    </row>
-    <row r="32" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="N32" s="13">
-        <v>0</v>
-      </c>
-      <c r="O32" s="9"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="15"/>
-    </row>
-    <row r="33" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N33" s="11">
-        <v>1</v>
-      </c>
-      <c r="O33" s="10"/>
+      <c r="S32" s="14"/>
+    </row>
+    <row r="33" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N33" s="12">
+        <v>0</v>
+      </c>
+      <c r="O33" s="8"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
       <c r="R33" s="5"/>
-      <c r="S33" s="15"/>
-    </row>
-    <row r="34" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S34" s="15"/>
+      <c r="S33" s="14"/>
+    </row>
+    <row r="34" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N34" s="10">
+        <v>1</v>
+      </c>
+      <c r="O34" s="9"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="14"/>
     </row>
     <row r="35" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S35" s="15"/>
-    </row>
-    <row r="36" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S36" s="15"/>
+      <c r="S35" s="14"/>
+    </row>
+    <row r="36" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="S36" s="14"/>
     </row>
     <row r="37" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N37" s="14" t="s">
+      <c r="S37" s="14"/>
+    </row>
+    <row r="38" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N38" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="O37" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P37" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="7" t="s">
+      <c r="O38" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="P38" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="R37" s="8" t="s">
+      <c r="R38" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="S37" s="15"/>
-    </row>
-    <row r="38" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N38" s="13">
-        <v>0</v>
-      </c>
-      <c r="O38" s="9"/>
-      <c r="P38" s="6"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
-      <c r="S38" s="15"/>
-    </row>
-    <row r="39" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N39" s="11">
-        <v>1</v>
-      </c>
-      <c r="O39" s="10"/>
+      <c r="S38" s="14"/>
+    </row>
+    <row r="39" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="N39" s="12">
+        <v>0</v>
+      </c>
+      <c r="O39" s="8"/>
       <c r="P39" s="5"/>
       <c r="Q39" s="5"/>
       <c r="R39" s="5"/>
-      <c r="S39" s="15"/>
-    </row>
-    <row r="40" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S40" s="15"/>
+      <c r="S39" s="14"/>
+    </row>
+    <row r="40" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N40" s="10">
+        <v>1</v>
+      </c>
+      <c r="O40" s="9"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="14"/>
     </row>
     <row r="41" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S41" s="15"/>
-    </row>
-    <row r="42" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S42" s="15"/>
-    </row>
-    <row r="43" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N43" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="O43" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="P43" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q43" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="R43" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="S43" s="15"/>
+      <c r="S41" s="14"/>
+    </row>
+    <row r="42" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="S42" s="14"/>
+    </row>
+    <row r="43" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="S43" s="14"/>
     </row>
     <row r="44" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N44" s="13">
-        <v>0</v>
-      </c>
-      <c r="O44" s="9"/>
-      <c r="P44" s="6"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
-      <c r="S44" s="15"/>
-    </row>
-    <row r="45" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N45" s="11">
-        <v>1</v>
-      </c>
-      <c r="O45" s="10"/>
-      <c r="P45" s="5"/>
-      <c r="Q45" s="5"/>
-      <c r="R45" s="5"/>
-      <c r="S45" s="15"/>
+      <c r="S44" s="14"/>
+    </row>
+    <row r="45" spans="14:19" x14ac:dyDescent="0.25">
+      <c r="S45" s="14"/>
     </row>
     <row r="46" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S46" s="15"/>
+      <c r="S46" s="14"/>
     </row>
     <row r="47" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S47" s="15"/>
+      <c r="S47" s="14"/>
     </row>
     <row r="48" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S48" s="15"/>
+      <c r="S48" s="14"/>
     </row>
     <row r="49" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S49" s="15"/>
+      <c r="S49" s="14"/>
     </row>
     <row r="50" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S50" s="15"/>
+      <c r="S50" s="14"/>
     </row>
     <row r="51" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S51" s="15"/>
+      <c r="S51" s="14"/>
     </row>
     <row r="52" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S52" s="15"/>
+      <c r="S52" s="14"/>
     </row>
     <row r="53" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S53" s="15"/>
+      <c r="S53" s="14"/>
     </row>
     <row r="54" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S54" s="15"/>
+      <c r="S54" s="14"/>
     </row>
     <row r="55" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S55" s="15"/>
+      <c r="S55" s="14"/>
     </row>
     <row r="56" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S56" s="15"/>
+      <c r="S56" s="14"/>
     </row>
     <row r="57" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S57" s="15"/>
+      <c r="S57" s="14"/>
     </row>
     <row r="58" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S58" s="15"/>
+      <c r="S58" s="14"/>
     </row>
     <row r="59" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S59" s="15"/>
+      <c r="S59" s="14"/>
     </row>
     <row r="60" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S60" s="15"/>
+      <c r="S60" s="14"/>
     </row>
     <row r="61" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S61" s="15"/>
+      <c r="S61" s="14"/>
     </row>
     <row r="62" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S62" s="15"/>
+      <c r="S62" s="14"/>
     </row>
     <row r="63" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S63" s="15"/>
+      <c r="S63" s="14"/>
     </row>
     <row r="64" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S64" s="15"/>
+      <c r="S64" s="14"/>
     </row>
     <row r="65" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S65" s="15"/>
+      <c r="S65" s="14"/>
     </row>
     <row r="66" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S66" s="15"/>
+      <c r="S66" s="14"/>
     </row>
     <row r="67" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S67" s="15"/>
+      <c r="S67" s="14"/>
     </row>
     <row r="68" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S68" s="15"/>
+      <c r="S68" s="14"/>
     </row>
     <row r="69" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S69" s="15"/>
+      <c r="S69" s="14"/>
     </row>
     <row r="70" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S70" s="15"/>
+      <c r="S70" s="14"/>
     </row>
     <row r="71" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S71" s="15"/>
+      <c r="S71" s="14"/>
     </row>
     <row r="72" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S72" s="15"/>
+      <c r="S72" s="14"/>
     </row>
     <row r="73" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S73" s="15"/>
+      <c r="S73" s="14"/>
     </row>
     <row r="74" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S74" s="15"/>
+      <c r="S74" s="14"/>
     </row>
     <row r="75" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S75" s="15"/>
+      <c r="S75" s="14"/>
     </row>
     <row r="76" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S76" s="15"/>
+      <c r="S76" s="14"/>
     </row>
     <row r="77" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S77" s="15"/>
+      <c r="S77" s="14"/>
     </row>
     <row r="78" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S78" s="15"/>
+      <c r="S78" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
se agregaron los mapas de karnaugh de anodo comun y el circuito de prueba
</commit_message>
<xml_diff>
--- a/mapas_de_karnaugh.xlsx
+++ b/mapas_de_karnaugh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoséSandoval\Desktop\P1_ORGA_G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81BC7BE-B8C5-46E6-8A63-72E9D150C75E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD552881-A758-41C9-8EF5-D49FF17E7BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0ECEB190-8471-4C0B-8113-5907E8DD918B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="33">
   <si>
     <t>00</t>
   </si>
@@ -120,6 +120,21 @@
   </si>
   <si>
     <t>F1 = yz' + x'z'</t>
+  </si>
+  <si>
+    <t>F1 = z + xy'</t>
+  </si>
+  <si>
+    <t>F2 = 0</t>
+  </si>
+  <si>
+    <t>F3 =  z'</t>
+  </si>
+  <si>
+    <t>PARA A, B Y F</t>
+  </si>
+  <si>
+    <t>PARA E, G</t>
   </si>
 </sst>
 </file>
@@ -142,7 +157,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,6 +188,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -324,12 +345,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -362,10 +380,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -378,6 +392,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,16 +420,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>5921</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>129746</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -438,7 +459,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="476250" y="2066925"/>
+          <a:off x="95250" y="4143375"/>
           <a:ext cx="2457450" cy="3387296"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -780,8 +801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC71AE7-27C8-4321-8A12-F43BE1CD410D}">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T21" sqref="T21"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,28 +830,28 @@
       <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="K1" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="L1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="14"/>
+      <c r="S1" s="13"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -848,31 +869,31 @@
       <c r="E2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="22">
-        <v>1</v>
-      </c>
-      <c r="G2" s="22">
-        <v>1</v>
-      </c>
-      <c r="H2" s="15">
-        <v>0</v>
-      </c>
-      <c r="I2" s="15">
-        <v>0</v>
-      </c>
-      <c r="J2" s="21">
-        <v>1</v>
-      </c>
-      <c r="K2" s="22">
-        <v>1</v>
-      </c>
-      <c r="L2" s="21">
+      <c r="F2" s="17">
+        <v>1</v>
+      </c>
+      <c r="G2" s="17">
+        <v>1</v>
+      </c>
+      <c r="H2" s="14">
+        <v>0</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0</v>
+      </c>
+      <c r="J2" s="16">
+        <v>1</v>
+      </c>
+      <c r="K2" s="17">
+        <v>1</v>
+      </c>
+      <c r="L2" s="16">
         <v>1</v>
       </c>
       <c r="N2" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="14"/>
+      <c r="S2" s="13"/>
     </row>
     <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -890,28 +911,28 @@
       <c r="E3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="22">
-        <v>0</v>
-      </c>
-      <c r="G3" s="22">
-        <v>0</v>
-      </c>
-      <c r="H3" s="15">
-        <v>1</v>
-      </c>
-      <c r="I3" s="15">
-        <v>1</v>
-      </c>
-      <c r="J3" s="21">
-        <v>1</v>
-      </c>
-      <c r="K3" s="22">
-        <v>0</v>
-      </c>
-      <c r="L3" s="21">
-        <v>1</v>
-      </c>
-      <c r="S3" s="14"/>
+      <c r="F3" s="17">
+        <v>0</v>
+      </c>
+      <c r="G3" s="17">
+        <v>0</v>
+      </c>
+      <c r="H3" s="14">
+        <v>1</v>
+      </c>
+      <c r="I3" s="14">
+        <v>1</v>
+      </c>
+      <c r="J3" s="16">
+        <v>1</v>
+      </c>
+      <c r="K3" s="17">
+        <v>0</v>
+      </c>
+      <c r="L3" s="16">
+        <v>1</v>
+      </c>
+      <c r="S3" s="13"/>
     </row>
     <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -929,43 +950,43 @@
       <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="G4" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="15">
-        <v>0</v>
-      </c>
-      <c r="J4" s="21">
-        <v>1</v>
-      </c>
-      <c r="K4" s="22">
-        <v>1</v>
-      </c>
-      <c r="L4" s="21">
-        <v>1</v>
-      </c>
-      <c r="N4" s="13" t="s">
+      <c r="I4" s="14">
+        <v>0</v>
+      </c>
+      <c r="J4" s="16">
+        <v>1</v>
+      </c>
+      <c r="K4" s="17">
+        <v>1</v>
+      </c>
+      <c r="L4" s="16">
+        <v>1</v>
+      </c>
+      <c r="N4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O4" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="6" t="s">
+      <c r="O4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="R4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S4" s="14"/>
+      <c r="S4" s="13"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -983,43 +1004,43 @@
       <c r="E5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="22">
-        <v>0</v>
-      </c>
-      <c r="G5" s="22">
-        <v>0</v>
-      </c>
-      <c r="H5" s="15">
-        <v>1</v>
-      </c>
-      <c r="I5" s="15">
-        <v>1</v>
-      </c>
-      <c r="J5" s="21">
-        <v>1</v>
-      </c>
-      <c r="K5" s="22">
-        <v>0</v>
-      </c>
-      <c r="L5" s="21">
-        <v>1</v>
-      </c>
-      <c r="N5" s="12">
-        <v>0</v>
-      </c>
-      <c r="O5" s="26">
-        <v>1</v>
-      </c>
-      <c r="P5" s="18">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="18">
-        <v>0</v>
-      </c>
-      <c r="R5" s="24">
-        <v>1</v>
-      </c>
-      <c r="S5" s="14"/>
+      <c r="F5" s="17">
+        <v>0</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0</v>
+      </c>
+      <c r="H5" s="14">
+        <v>1</v>
+      </c>
+      <c r="I5" s="14">
+        <v>1</v>
+      </c>
+      <c r="J5" s="16">
+        <v>1</v>
+      </c>
+      <c r="K5" s="17">
+        <v>0</v>
+      </c>
+      <c r="L5" s="16">
+        <v>1</v>
+      </c>
+      <c r="N5" s="11">
+        <v>0</v>
+      </c>
+      <c r="O5" s="21">
+        <v>1</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0</v>
+      </c>
+      <c r="R5" s="19">
+        <v>1</v>
+      </c>
+      <c r="S5" s="13"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -1037,43 +1058,43 @@
       <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="22">
-        <v>0</v>
-      </c>
-      <c r="G6" s="22">
-        <v>0</v>
-      </c>
-      <c r="H6" s="15">
-        <v>0</v>
-      </c>
-      <c r="I6" s="15">
-        <v>0</v>
-      </c>
-      <c r="J6" s="21">
-        <v>1</v>
-      </c>
-      <c r="K6" s="22">
-        <v>0</v>
-      </c>
-      <c r="L6" s="21">
-        <v>1</v>
-      </c>
-      <c r="N6" s="10">
-        <v>1</v>
-      </c>
-      <c r="O6" s="19">
-        <v>0</v>
-      </c>
-      <c r="P6" s="20">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="20">
-        <v>0</v>
-      </c>
-      <c r="R6" s="25">
-        <v>1</v>
-      </c>
-      <c r="S6" s="14" t="s">
+      <c r="F6" s="17">
+        <v>0</v>
+      </c>
+      <c r="G6" s="17">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0</v>
+      </c>
+      <c r="J6" s="16">
+        <v>1</v>
+      </c>
+      <c r="K6" s="17">
+        <v>0</v>
+      </c>
+      <c r="L6" s="16">
+        <v>1</v>
+      </c>
+      <c r="N6" s="9">
+        <v>1</v>
+      </c>
+      <c r="O6" s="8">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0</v>
+      </c>
+      <c r="R6" s="20">
+        <v>1</v>
+      </c>
+      <c r="S6" s="13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1093,28 +1114,28 @@
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="22">
-        <v>0</v>
-      </c>
-      <c r="G7" s="22">
-        <v>0</v>
-      </c>
-      <c r="H7" s="15">
-        <v>1</v>
-      </c>
-      <c r="I7" s="15">
-        <v>1</v>
-      </c>
-      <c r="J7" s="21">
-        <v>1</v>
-      </c>
-      <c r="K7" s="22">
-        <v>0</v>
-      </c>
-      <c r="L7" s="21">
-        <v>1</v>
-      </c>
-      <c r="S7" s="14"/>
+      <c r="F7" s="17">
+        <v>0</v>
+      </c>
+      <c r="G7" s="17">
+        <v>0</v>
+      </c>
+      <c r="H7" s="14">
+        <v>1</v>
+      </c>
+      <c r="I7" s="14">
+        <v>1</v>
+      </c>
+      <c r="J7" s="16">
+        <v>1</v>
+      </c>
+      <c r="K7" s="17">
+        <v>0</v>
+      </c>
+      <c r="L7" s="16">
+        <v>1</v>
+      </c>
+      <c r="S7" s="13"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -1132,31 +1153,31 @@
       <c r="E8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="22">
-        <v>1</v>
-      </c>
-      <c r="G8" s="22">
-        <v>1</v>
-      </c>
-      <c r="H8" s="15">
-        <v>0</v>
-      </c>
-      <c r="I8" s="15">
-        <v>0</v>
-      </c>
-      <c r="J8" s="21">
-        <v>1</v>
-      </c>
-      <c r="K8" s="22">
-        <v>1</v>
-      </c>
-      <c r="L8" s="21">
+      <c r="F8" s="17">
+        <v>1</v>
+      </c>
+      <c r="G8" s="17">
+        <v>1</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14">
+        <v>0</v>
+      </c>
+      <c r="J8" s="16">
+        <v>1</v>
+      </c>
+      <c r="K8" s="17">
+        <v>1</v>
+      </c>
+      <c r="L8" s="16">
         <v>1</v>
       </c>
       <c r="N8" t="s">
         <v>23</v>
       </c>
-      <c r="S8" s="14"/>
+      <c r="S8" s="13"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -1174,439 +1195,816 @@
       <c r="E9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="22">
-        <v>0</v>
-      </c>
-      <c r="G9" s="22">
-        <v>0</v>
-      </c>
-      <c r="H9" s="15">
-        <v>1</v>
-      </c>
-      <c r="I9" s="15">
-        <v>1</v>
-      </c>
-      <c r="J9" s="21">
-        <v>1</v>
-      </c>
-      <c r="K9" s="22">
-        <v>0</v>
-      </c>
-      <c r="L9" s="21">
-        <v>1</v>
-      </c>
-      <c r="S9" s="14"/>
+      <c r="F9" s="17">
+        <v>0</v>
+      </c>
+      <c r="G9" s="17">
+        <v>0</v>
+      </c>
+      <c r="H9" s="14">
+        <v>1</v>
+      </c>
+      <c r="I9" s="14">
+        <v>1</v>
+      </c>
+      <c r="J9" s="16">
+        <v>1</v>
+      </c>
+      <c r="K9" s="17">
+        <v>0</v>
+      </c>
+      <c r="L9" s="16">
+        <v>1</v>
+      </c>
+      <c r="S9" s="13"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N10" s="13" t="s">
+      <c r="N10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O10" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P10" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q10" s="6" t="s">
+      <c r="O10" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="R10" s="7" t="s">
+      <c r="R10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S10" s="14"/>
+      <c r="S10" s="13"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="N11" s="12">
-        <v>0</v>
-      </c>
-      <c r="O11" s="17">
-        <v>0</v>
-      </c>
-      <c r="P11" s="24">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="24">
-        <v>1</v>
-      </c>
-      <c r="R11" s="18">
-        <v>0</v>
-      </c>
-      <c r="S11" s="14" t="s">
+      <c r="N11" s="11">
+        <v>0</v>
+      </c>
+      <c r="O11" s="7">
+        <v>0</v>
+      </c>
+      <c r="P11" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="19">
+        <v>1</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0</v>
+      </c>
+      <c r="S11" s="13" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N12" s="10">
-        <v>1</v>
-      </c>
-      <c r="O12" s="19">
-        <v>0</v>
-      </c>
-      <c r="P12" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="25">
-        <v>1</v>
-      </c>
-      <c r="R12" s="20">
-        <v>0</v>
-      </c>
-      <c r="S12" s="14"/>
+      <c r="N12" s="9">
+        <v>1</v>
+      </c>
+      <c r="O12" s="8">
+        <v>0</v>
+      </c>
+      <c r="P12" s="20">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="20">
+        <v>1</v>
+      </c>
+      <c r="R12" s="3">
+        <v>0</v>
+      </c>
+      <c r="S12" s="13"/>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S13" s="14"/>
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="S13" s="13"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="17">
+        <v>0</v>
+      </c>
+      <c r="G14" s="17">
+        <v>0</v>
+      </c>
+      <c r="H14" s="14">
+        <v>1</v>
+      </c>
+      <c r="I14" s="14">
+        <v>1</v>
+      </c>
+      <c r="J14" s="16">
+        <v>0</v>
+      </c>
+      <c r="K14" s="17">
+        <v>0</v>
+      </c>
+      <c r="L14" s="16">
+        <v>0</v>
+      </c>
       <c r="N14" t="s">
         <v>24</v>
       </c>
-      <c r="S14" s="14"/>
+      <c r="S14" s="13"/>
     </row>
     <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S15" s="14"/>
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="17">
+        <v>1</v>
+      </c>
+      <c r="G15" s="17">
+        <v>1</v>
+      </c>
+      <c r="H15" s="14">
+        <v>0</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0</v>
+      </c>
+      <c r="J15" s="16">
+        <v>0</v>
+      </c>
+      <c r="K15" s="17">
+        <v>1</v>
+      </c>
+      <c r="L15" s="16">
+        <v>0</v>
+      </c>
+      <c r="S15" s="13"/>
     </row>
     <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N16" s="13" t="s">
+      <c r="A16" s="1">
         <v>2</v>
       </c>
-      <c r="O16" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P16" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="6" t="s">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="14">
+        <v>1</v>
+      </c>
+      <c r="J16" s="16">
+        <v>0</v>
+      </c>
+      <c r="K16" s="17">
+        <v>0</v>
+      </c>
+      <c r="L16" s="16">
+        <v>0</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="O16" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P16" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="R16" s="7" t="s">
+      <c r="R16" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S16" s="14"/>
-    </row>
-    <row r="17" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G17" s="1"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="N17" s="12">
-        <v>0</v>
-      </c>
-      <c r="O17" s="17">
-        <v>1</v>
-      </c>
-      <c r="P17" s="18">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="18">
-        <v>1</v>
-      </c>
-      <c r="R17" s="18">
-        <v>1</v>
-      </c>
-      <c r="S17" s="14" t="s">
+      <c r="S16" s="13"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="17">
+        <v>1</v>
+      </c>
+      <c r="G17" s="17">
+        <v>1</v>
+      </c>
+      <c r="H17" s="14">
+        <v>0</v>
+      </c>
+      <c r="I17" s="14">
+        <v>0</v>
+      </c>
+      <c r="J17" s="16">
+        <v>0</v>
+      </c>
+      <c r="K17" s="17">
+        <v>1</v>
+      </c>
+      <c r="L17" s="16">
+        <v>0</v>
+      </c>
+      <c r="N17" s="11">
+        <v>0</v>
+      </c>
+      <c r="O17" s="7">
+        <v>1</v>
+      </c>
+      <c r="P17" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>1</v>
+      </c>
+      <c r="R17" s="4">
+        <v>1</v>
+      </c>
+      <c r="S17" s="13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G18" s="1"/>
-      <c r="N18" s="10">
-        <v>1</v>
-      </c>
-      <c r="O18" s="19">
-        <v>1</v>
-      </c>
-      <c r="P18" s="20">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="20">
-        <v>1</v>
-      </c>
-      <c r="R18" s="20">
-        <v>1</v>
-      </c>
-      <c r="S18" s="14"/>
-    </row>
-    <row r="19" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="G19" s="1"/>
-      <c r="S19" s="14"/>
-    </row>
-    <row r="20" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="S20" s="14"/>
-    </row>
-    <row r="21" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="N21" s="3"/>
-      <c r="O21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="14"/>
-    </row>
-    <row r="22" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="N22" s="3"/>
-      <c r="O22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="14"/>
-    </row>
-    <row r="23" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="S23" s="14"/>
-    </row>
-    <row r="24" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="S24" s="14"/>
-    </row>
-    <row r="25" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S25" s="14"/>
-    </row>
-    <row r="26" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N26" s="13" t="s">
+    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="17">
+        <v>1</v>
+      </c>
+      <c r="G18" s="17">
+        <v>1</v>
+      </c>
+      <c r="H18" s="14">
+        <v>1</v>
+      </c>
+      <c r="I18" s="14">
+        <v>1</v>
+      </c>
+      <c r="J18" s="16">
+        <v>0</v>
+      </c>
+      <c r="K18" s="17">
+        <v>1</v>
+      </c>
+      <c r="L18" s="16">
+        <v>0</v>
+      </c>
+      <c r="N18" s="9">
+        <v>1</v>
+      </c>
+      <c r="O18" s="8">
+        <v>1</v>
+      </c>
+      <c r="P18" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>1</v>
+      </c>
+      <c r="R18" s="3">
+        <v>1</v>
+      </c>
+      <c r="S18" s="13"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1">
+        <v>1</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="17">
+        <v>1</v>
+      </c>
+      <c r="G19" s="17">
+        <v>1</v>
+      </c>
+      <c r="H19" s="14">
+        <v>0</v>
+      </c>
+      <c r="I19" s="14">
+        <v>0</v>
+      </c>
+      <c r="J19" s="16">
+        <v>0</v>
+      </c>
+      <c r="K19" s="17">
+        <v>1</v>
+      </c>
+      <c r="L19" s="16">
+        <v>0</v>
+      </c>
+      <c r="S19" s="13"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>6</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0</v>
+      </c>
+      <c r="G20" s="17">
+        <v>0</v>
+      </c>
+      <c r="H20" s="14">
+        <v>1</v>
+      </c>
+      <c r="I20" s="14">
+        <v>1</v>
+      </c>
+      <c r="J20" s="16">
+        <v>0</v>
+      </c>
+      <c r="K20" s="17">
+        <v>0</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0</v>
+      </c>
+      <c r="S20" s="13"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>7</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="17">
+        <v>1</v>
+      </c>
+      <c r="G21" s="17">
+        <v>1</v>
+      </c>
+      <c r="H21" s="14">
+        <v>0</v>
+      </c>
+      <c r="I21" s="14">
+        <v>0</v>
+      </c>
+      <c r="J21" s="16">
+        <v>0</v>
+      </c>
+      <c r="K21" s="17">
+        <v>1</v>
+      </c>
+      <c r="L21" s="16">
+        <v>0</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="13"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="13"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S23" s="13"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N24" t="s">
+        <v>31</v>
+      </c>
+      <c r="S24" s="13"/>
+    </row>
+    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S25" s="13"/>
+    </row>
+    <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N26" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O26" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P26" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="6" t="s">
+      <c r="O26" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P26" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="R26" s="7" t="s">
+      <c r="R26" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S26" s="14"/>
-    </row>
-    <row r="27" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="N27" s="12">
-        <v>0</v>
-      </c>
-      <c r="O27" s="8"/>
-      <c r="P27" s="5"/>
-      <c r="Q27" s="5"/>
-      <c r="R27" s="5"/>
-      <c r="S27" s="14"/>
-    </row>
-    <row r="28" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N28" s="10">
-        <v>1</v>
-      </c>
-      <c r="O28" s="9"/>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
-      <c r="R28" s="4"/>
-      <c r="S28" s="14"/>
-    </row>
-    <row r="29" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="S29" s="14"/>
-    </row>
-    <row r="30" spans="7:19" x14ac:dyDescent="0.25">
-      <c r="S30" s="14"/>
-    </row>
-    <row r="31" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S31" s="14"/>
-    </row>
-    <row r="32" spans="7:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N32" s="13" t="s">
+      <c r="S26" s="13"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N27" s="11">
+        <v>0</v>
+      </c>
+      <c r="O27" s="7">
+        <v>0</v>
+      </c>
+      <c r="P27" s="22">
+        <v>1</v>
+      </c>
+      <c r="Q27" s="22">
+        <v>1</v>
+      </c>
+      <c r="R27" s="4">
+        <v>0</v>
+      </c>
+      <c r="S27" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N28" s="9">
+        <v>1</v>
+      </c>
+      <c r="O28" s="24">
+        <v>1</v>
+      </c>
+      <c r="P28" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="23">
+        <v>1</v>
+      </c>
+      <c r="R28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="S29" s="13"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>32</v>
+      </c>
+      <c r="S30" s="13"/>
+    </row>
+    <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="S31" s="13"/>
+    </row>
+    <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N32" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O32" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P32" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q32" s="6" t="s">
+      <c r="O32" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P32" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q32" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="R32" s="7" t="s">
+      <c r="R32" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S32" s="14"/>
+      <c r="S32" s="13"/>
     </row>
     <row r="33" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N33" s="12">
-        <v>0</v>
-      </c>
-      <c r="O33" s="8"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="5"/>
-      <c r="R33" s="5"/>
-      <c r="S33" s="14"/>
+      <c r="N33" s="11">
+        <v>0</v>
+      </c>
+      <c r="O33" s="7">
+        <v>0</v>
+      </c>
+      <c r="P33" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="4">
+        <v>0</v>
+      </c>
+      <c r="R33" s="4">
+        <v>0</v>
+      </c>
+      <c r="S33" s="13" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="34" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N34" s="10">
-        <v>1</v>
-      </c>
-      <c r="O34" s="9"/>
-      <c r="P34" s="4"/>
-      <c r="Q34" s="4"/>
-      <c r="R34" s="4"/>
-      <c r="S34" s="14"/>
+      <c r="N34" s="9">
+        <v>1</v>
+      </c>
+      <c r="O34" s="8">
+        <v>0</v>
+      </c>
+      <c r="P34" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>0</v>
+      </c>
+      <c r="R34" s="3">
+        <v>0</v>
+      </c>
+      <c r="S34" s="13"/>
     </row>
     <row r="35" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S35" s="14"/>
+      <c r="S35" s="13"/>
     </row>
     <row r="36" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S36" s="14"/>
+      <c r="S36" s="13"/>
     </row>
     <row r="37" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S37" s="14"/>
+      <c r="S37" s="13"/>
     </row>
     <row r="38" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N38" s="13" t="s">
+      <c r="N38" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="O38" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="P38" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q38" s="6" t="s">
+      <c r="O38" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P38" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="R38" s="7" t="s">
+      <c r="R38" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="S38" s="14"/>
+      <c r="S38" s="13"/>
     </row>
     <row r="39" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="N39" s="12">
-        <v>0</v>
-      </c>
-      <c r="O39" s="8"/>
-      <c r="P39" s="5"/>
-      <c r="Q39" s="5"/>
-      <c r="R39" s="5"/>
-      <c r="S39" s="14"/>
+      <c r="N39" s="11">
+        <v>0</v>
+      </c>
+      <c r="O39" s="21">
+        <v>1</v>
+      </c>
+      <c r="P39" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>0</v>
+      </c>
+      <c r="R39" s="27">
+        <v>1</v>
+      </c>
+      <c r="S39" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="40" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N40" s="10">
-        <v>1</v>
-      </c>
-      <c r="O40" s="9"/>
-      <c r="P40" s="4"/>
-      <c r="Q40" s="4"/>
-      <c r="R40" s="4"/>
-      <c r="S40" s="14"/>
+      <c r="N40" s="9">
+        <v>1</v>
+      </c>
+      <c r="O40" s="26">
+        <v>1</v>
+      </c>
+      <c r="P40" s="3">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>0</v>
+      </c>
+      <c r="R40" s="28">
+        <v>1</v>
+      </c>
+      <c r="S40" s="13"/>
     </row>
     <row r="41" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S41" s="14"/>
+      <c r="S41" s="13"/>
     </row>
     <row r="42" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S42" s="14"/>
+      <c r="S42" s="13"/>
     </row>
     <row r="43" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S43" s="14"/>
+      <c r="S43" s="13"/>
     </row>
     <row r="44" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S44" s="14"/>
+      <c r="S44" s="13"/>
     </row>
     <row r="45" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S45" s="14"/>
+      <c r="S45" s="13"/>
     </row>
     <row r="46" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S46" s="14"/>
+      <c r="S46" s="13"/>
     </row>
     <row r="47" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S47" s="14"/>
+      <c r="S47" s="13"/>
     </row>
     <row r="48" spans="14:19" x14ac:dyDescent="0.25">
-      <c r="S48" s="14"/>
+      <c r="S48" s="13"/>
     </row>
     <row r="49" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S49" s="14"/>
+      <c r="S49" s="13"/>
     </row>
     <row r="50" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S50" s="14"/>
+      <c r="S50" s="13"/>
     </row>
     <row r="51" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S51" s="14"/>
+      <c r="S51" s="13"/>
     </row>
     <row r="52" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S52" s="14"/>
+      <c r="S52" s="13"/>
     </row>
     <row r="53" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S53" s="14"/>
+      <c r="S53" s="13"/>
     </row>
     <row r="54" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S54" s="14"/>
+      <c r="S54" s="13"/>
     </row>
     <row r="55" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S55" s="14"/>
+      <c r="S55" s="13"/>
     </row>
     <row r="56" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S56" s="14"/>
+      <c r="S56" s="13"/>
     </row>
     <row r="57" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S57" s="14"/>
+      <c r="S57" s="13"/>
     </row>
     <row r="58" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S58" s="14"/>
+      <c r="S58" s="13"/>
     </row>
     <row r="59" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S59" s="14"/>
+      <c r="S59" s="13"/>
     </row>
     <row r="60" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S60" s="14"/>
+      <c r="S60" s="13"/>
     </row>
     <row r="61" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S61" s="14"/>
+      <c r="S61" s="13"/>
     </row>
     <row r="62" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S62" s="14"/>
+      <c r="S62" s="13"/>
     </row>
     <row r="63" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S63" s="14"/>
+      <c r="S63" s="13"/>
     </row>
     <row r="64" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S64" s="14"/>
+      <c r="S64" s="13"/>
     </row>
     <row r="65" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S65" s="14"/>
+      <c r="S65" s="13"/>
     </row>
     <row r="66" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S66" s="14"/>
+      <c r="S66" s="13"/>
     </row>
     <row r="67" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S67" s="14"/>
+      <c r="S67" s="13"/>
     </row>
     <row r="68" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S68" s="14"/>
+      <c r="S68" s="13"/>
     </row>
     <row r="69" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S69" s="14"/>
+      <c r="S69" s="13"/>
     </row>
     <row r="70" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S70" s="14"/>
+      <c r="S70" s="13"/>
     </row>
     <row r="71" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S71" s="14"/>
+      <c r="S71" s="13"/>
     </row>
     <row r="72" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S72" s="14"/>
+      <c r="S72" s="13"/>
     </row>
     <row r="73" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S73" s="14"/>
+      <c r="S73" s="13"/>
     </row>
     <row r="74" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S74" s="14"/>
+      <c r="S74" s="13"/>
     </row>
     <row r="75" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S75" s="14"/>
+      <c r="S75" s="13"/>
     </row>
     <row r="76" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S76" s="14"/>
+      <c r="S76" s="13"/>
     </row>
     <row r="77" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S77" s="14"/>
+      <c r="S77" s="13"/>
     </row>
     <row r="78" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S78" s="14"/>
+      <c r="S78" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cambios hechos a las 2 am en la parte del catodo comun,
</commit_message>
<xml_diff>
--- a/mapas_de_karnaugh.xlsx
+++ b/mapas_de_karnaugh.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban Sánchez\Documents\GitHub\ORGA\P1_ORGA_G3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARROQUIN\Documents\yon\Quinto semestre\LAB ORGA\P1_ORGA_G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D245909A-C35E-45C5-B171-0DD48ECD310A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEBC470-1244-493D-99E9-DB44FC190256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0ECEB190-8471-4C0B-8113-5907E8DD918B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0ECEB190-8471-4C0B-8113-5907E8DD918B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -122,9 +122,6 @@
     <t>F1 = yz' + x'z'</t>
   </si>
   <si>
-    <t>F1 = z + xy'</t>
-  </si>
-  <si>
     <t>F2 = 0</t>
   </si>
   <si>
@@ -138,6 +135,9 @@
   </si>
   <si>
     <t>PARA C, D</t>
+  </si>
+  <si>
+    <t>F1 = (x'+y)(z')</t>
   </si>
 </sst>
 </file>
@@ -193,7 +193,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -348,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,13 +395,19 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -804,20 +810,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC71AE7-27C8-4321-8A12-F43BE1CD410D}">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" customWidth="1"/>
     <col min="2" max="2" width="5" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" customWidth="1"/>
     <col min="6" max="12" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -856,7 +862,7 @@
       </c>
       <c r="S1" s="13"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -898,7 +904,7 @@
       </c>
       <c r="S2" s="13"/>
     </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -937,7 +943,7 @@
       </c>
       <c r="S3" s="13"/>
     </row>
-    <row r="4" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -991,7 +997,7 @@
       </c>
       <c r="S4" s="13"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1045,7 +1051,7 @@
       </c>
       <c r="S5" s="13"/>
     </row>
-    <row r="6" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1140,7 +1146,7 @@
       </c>
       <c r="S7" s="13"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1182,7 +1188,7 @@
       </c>
       <c r="S8" s="13"/>
     </row>
-    <row r="9" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1221,7 +1227,7 @@
       </c>
       <c r="S9" s="13"/>
     </row>
-    <row r="10" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N10" s="12" t="s">
         <v>2</v>
       </c>
@@ -1239,7 +1245,7 @@
       </c>
       <c r="S10" s="13"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="N11" s="11">
         <v>0</v>
       </c>
@@ -1259,7 +1265,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N12" s="9">
         <v>1</v>
       </c>
@@ -1277,7 +1283,7 @@
       </c>
       <c r="S12" s="13"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>3</v>
       </c>
@@ -1316,7 +1322,7 @@
       </c>
       <c r="S13" s="13"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>0</v>
       </c>
@@ -1333,32 +1339,32 @@
         <v>15</v>
       </c>
       <c r="F14" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" t="s">
         <v>24</v>
       </c>
       <c r="S14" s="13"/>
     </row>
-    <row r="15" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -1375,29 +1381,29 @@
         <v>16</v>
       </c>
       <c r="F15" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S15" s="13"/>
     </row>
-    <row r="16" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>2</v>
       </c>
@@ -1414,25 +1420,25 @@
         <v>15</v>
       </c>
       <c r="F16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="G16" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>18</v>
-      </c>
       <c r="I16" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="12" t="s">
         <v>2</v>
@@ -1451,7 +1457,7 @@
       </c>
       <c r="S16" s="13"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>3</v>
       </c>
@@ -1468,25 +1474,25 @@
         <v>16</v>
       </c>
       <c r="F17" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G17" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J17" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L17" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N17" s="11">
         <v>0</v>
@@ -1507,7 +1513,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -1524,25 +1530,25 @@
         <v>17</v>
       </c>
       <c r="F18" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H18" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I18" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N18" s="9">
         <v>1</v>
@@ -1561,7 +1567,7 @@
       </c>
       <c r="S18" s="13"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>5</v>
       </c>
@@ -1578,29 +1584,29 @@
         <v>16</v>
       </c>
       <c r="F19" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L19" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" s="13"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>6</v>
       </c>
@@ -1617,29 +1623,29 @@
         <v>15</v>
       </c>
       <c r="F20" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I20" s="14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20" s="13"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>7</v>
       </c>
@@ -1656,25 +1662,25 @@
         <v>16</v>
       </c>
       <c r="F21" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G21" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I21" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L21" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
@@ -1683,7 +1689,7 @@
       <c r="R21" s="2"/>
       <c r="S21" s="13"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
@@ -1691,19 +1697,19 @@
       <c r="R22" s="2"/>
       <c r="S22" s="13"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="S23" s="13"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="N24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S24" s="13"/>
     </row>
-    <row r="25" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="S25" s="13"/>
     </row>
-    <row r="26" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N26" s="12" t="s">
         <v>2</v>
       </c>
@@ -1721,56 +1727,56 @@
       </c>
       <c r="S26" s="13"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
       <c r="N27" s="11">
         <v>0</v>
       </c>
-      <c r="O27" s="7">
-        <v>0</v>
-      </c>
-      <c r="P27" s="22">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="22">
-        <v>1</v>
-      </c>
-      <c r="R27" s="4">
-        <v>0</v>
+      <c r="O27" s="22">
+        <v>1</v>
+      </c>
+      <c r="P27" s="27">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="27">
+        <v>0</v>
+      </c>
+      <c r="R27" s="23">
+        <v>1</v>
       </c>
       <c r="S27" s="13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N28" s="9">
         <v>1</v>
       </c>
-      <c r="O28" s="24">
-        <v>1</v>
-      </c>
-      <c r="P28" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="23">
-        <v>1</v>
-      </c>
-      <c r="R28" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="O28" s="29">
+        <v>0</v>
+      </c>
+      <c r="P28" s="30">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="28">
+        <v>0</v>
+      </c>
+      <c r="R28" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
       <c r="S29" s="13"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
       <c r="N30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S30" s="13"/>
     </row>
-    <row r="31" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="S31" s="13"/>
     </row>
-    <row r="32" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N32" s="12" t="s">
         <v>2</v>
       </c>
@@ -1788,57 +1794,57 @@
       </c>
       <c r="S32" s="13"/>
     </row>
-    <row r="33" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N33" s="11">
         <v>0</v>
       </c>
       <c r="O33" s="7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R33" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S33" s="13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="14:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N34" s="9">
         <v>1</v>
       </c>
       <c r="O34" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R34" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S34" s="13"/>
     </row>
-    <row r="35" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S35" s="13"/>
     </row>
-    <row r="36" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S36" s="13"/>
     </row>
-    <row r="37" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="14:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S37" s="13"/>
     </row>
-    <row r="38" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="14:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N38" s="12" t="s">
         <v>2</v>
       </c>
@@ -1856,161 +1862,161 @@
       </c>
       <c r="S38" s="13"/>
     </row>
-    <row r="39" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="14:19" x14ac:dyDescent="0.3">
       <c r="N39" s="11">
         <v>0</v>
       </c>
-      <c r="O39" s="21">
-        <v>1</v>
-      </c>
-      <c r="P39" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="4">
-        <v>0</v>
-      </c>
-      <c r="R39" s="27">
-        <v>1</v>
+      <c r="O39" s="31">
+        <v>0</v>
+      </c>
+      <c r="P39" s="25">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="25">
+        <v>1</v>
+      </c>
+      <c r="R39" s="33">
+        <v>0</v>
       </c>
       <c r="S39" s="13" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="14:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="14:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N40" s="9">
         <v>1</v>
       </c>
-      <c r="O40" s="26">
-        <v>1</v>
-      </c>
-      <c r="P40" s="3">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="3">
-        <v>0</v>
-      </c>
-      <c r="R40" s="28">
-        <v>1</v>
+      <c r="O40" s="32">
+        <v>0</v>
+      </c>
+      <c r="P40" s="26">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="26">
+        <v>1</v>
+      </c>
+      <c r="R40" s="34">
+        <v>0</v>
       </c>
       <c r="S40" s="13"/>
     </row>
-    <row r="41" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S41" s="13"/>
     </row>
-    <row r="42" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S42" s="13"/>
     </row>
-    <row r="43" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S43" s="13"/>
     </row>
-    <row r="44" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S44" s="13"/>
     </row>
-    <row r="45" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S45" s="13"/>
     </row>
-    <row r="46" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S46" s="13"/>
     </row>
-    <row r="47" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S47" s="13"/>
     </row>
-    <row r="48" spans="14:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S48" s="13"/>
     </row>
-    <row r="49" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S49" s="13"/>
     </row>
-    <row r="50" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S50" s="13"/>
     </row>
-    <row r="51" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S51" s="13"/>
     </row>
-    <row r="52" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S52" s="13"/>
     </row>
-    <row r="53" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S53" s="13"/>
     </row>
-    <row r="54" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S54" s="13"/>
     </row>
-    <row r="55" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S55" s="13"/>
     </row>
-    <row r="56" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S56" s="13"/>
     </row>
-    <row r="57" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S57" s="13"/>
     </row>
-    <row r="58" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S58" s="13"/>
     </row>
-    <row r="59" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S59" s="13"/>
     </row>
-    <row r="60" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S60" s="13"/>
     </row>
-    <row r="61" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S61" s="13"/>
     </row>
-    <row r="62" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S62" s="13"/>
     </row>
-    <row r="63" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S63" s="13"/>
     </row>
-    <row r="64" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S64" s="13"/>
     </row>
-    <row r="65" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S65" s="13"/>
     </row>
-    <row r="66" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S66" s="13"/>
     </row>
-    <row r="67" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S67" s="13"/>
     </row>
-    <row r="68" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S68" s="13"/>
     </row>
-    <row r="69" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S69" s="13"/>
     </row>
-    <row r="70" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S70" s="13"/>
     </row>
-    <row r="71" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S71" s="13"/>
     </row>
-    <row r="72" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S72" s="13"/>
     </row>
-    <row r="73" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S73" s="13"/>
     </row>
-    <row r="74" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S74" s="13"/>
     </row>
-    <row r="75" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S75" s="13"/>
     </row>
-    <row r="76" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S76" s="13"/>
     </row>
-    <row r="77" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S77" s="13"/>
     </row>
-    <row r="78" spans="19:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="19:19" x14ac:dyDescent="0.3">
       <c r="S78" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ya funciona el anodo comun solo falta transistores
</commit_message>
<xml_diff>
--- a/mapas_de_karnaugh.xlsx
+++ b/mapas_de_karnaugh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARROQUIN\Documents\yon\Quinto semestre\LAB ORGA\P1_ORGA_G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEBC470-1244-493D-99E9-DB44FC190256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF23265A-13C7-4848-B655-A42375FC9101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0ECEB190-8471-4C0B-8113-5907E8DD918B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
   <si>
     <t>00</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>F1 = (x'+y)(z')</t>
+  </si>
+  <si>
+    <t>F1= (x*y')+z</t>
   </si>
 </sst>
 </file>
@@ -348,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -395,19 +398,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -810,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC71AE7-27C8-4321-8A12-F43BE1CD410D}">
   <dimension ref="A1:S78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W35" sqref="W35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,16 +1726,16 @@
       <c r="N27" s="11">
         <v>0</v>
       </c>
-      <c r="O27" s="22">
-        <v>1</v>
-      </c>
-      <c r="P27" s="27">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="27">
-        <v>0</v>
-      </c>
-      <c r="R27" s="23">
+      <c r="O27" s="7">
+        <v>1</v>
+      </c>
+      <c r="P27" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="22">
+        <v>0</v>
+      </c>
+      <c r="R27" s="4">
         <v>1</v>
       </c>
       <c r="S27" s="13" t="s">
@@ -1751,17 +1746,20 @@
       <c r="N28" s="9">
         <v>1</v>
       </c>
-      <c r="O28" s="29">
-        <v>0</v>
-      </c>
-      <c r="P28" s="30">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="28">
-        <v>0</v>
-      </c>
-      <c r="R28" s="24">
-        <v>1</v>
+      <c r="O28" s="24">
+        <v>0</v>
+      </c>
+      <c r="P28" s="20">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="23">
+        <v>0</v>
+      </c>
+      <c r="R28" s="3">
+        <v>1</v>
+      </c>
+      <c r="S28" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
@@ -1866,16 +1864,16 @@
       <c r="N39" s="11">
         <v>0</v>
       </c>
-      <c r="O39" s="31">
-        <v>0</v>
-      </c>
-      <c r="P39" s="25">
-        <v>1</v>
-      </c>
-      <c r="Q39" s="25">
-        <v>1</v>
-      </c>
-      <c r="R39" s="33">
+      <c r="O39" s="25">
+        <v>0</v>
+      </c>
+      <c r="P39" s="4">
+        <v>1</v>
+      </c>
+      <c r="Q39" s="4">
+        <v>1</v>
+      </c>
+      <c r="R39" s="22">
         <v>0</v>
       </c>
       <c r="S39" s="13" t="s">
@@ -1886,16 +1884,16 @@
       <c r="N40" s="9">
         <v>1</v>
       </c>
-      <c r="O40" s="32">
-        <v>0</v>
-      </c>
-      <c r="P40" s="26">
-        <v>1</v>
-      </c>
-      <c r="Q40" s="26">
-        <v>1</v>
-      </c>
-      <c r="R40" s="34">
+      <c r="O40" s="26">
+        <v>0</v>
+      </c>
+      <c r="P40" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>1</v>
+      </c>
+      <c r="R40" s="23">
         <v>0</v>
       </c>
       <c r="S40" s="13"/>

</xml_diff>

<commit_message>
anodo comun ahora si funcional, shet
</commit_message>
<xml_diff>
--- a/mapas_de_karnaugh.xlsx
+++ b/mapas_de_karnaugh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MARROQUIN\Documents\yon\Quinto semestre\LAB ORGA\P1_ORGA_G3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE7F29E-C4E3-40FD-BD7D-35201D3595EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40B5201-4054-4C14-AA03-0B2170B07E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0ECEB190-8471-4C0B-8113-5907E8DD918B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="37">
   <si>
     <t>00</t>
   </si>
@@ -122,12 +122,6 @@
     <t>F1 = yz' + x'z'</t>
   </si>
   <si>
-    <t>F2 = 0</t>
-  </si>
-  <si>
-    <t>F3 =  z'</t>
-  </si>
-  <si>
     <t>PARA A, B Y F</t>
   </si>
   <si>
@@ -140,14 +134,26 @@
     <t>F1 = (x'+y)(z')</t>
   </si>
   <si>
-    <t>F1= (x*y')+z</t>
+    <t>Anodo comun</t>
+  </si>
+  <si>
+    <t>catodo comun</t>
+  </si>
+  <si>
+    <t>F2 = 1</t>
+  </si>
+  <si>
+    <t>F3 =  z</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +164,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -351,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -403,6 +416,11 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,7 +451,7 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>361950</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>129746</xdr:rowOff>
+      <xdr:rowOff>115791</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -803,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC71AE7-27C8-4321-8A12-F43BE1CD410D}">
-  <dimension ref="A1:S78"/>
+  <dimension ref="A1:AA78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,6 +834,8 @@
     <col min="3" max="3" width="5.44140625" customWidth="1"/>
     <col min="4" max="4" width="4.88671875" customWidth="1"/>
     <col min="6" max="12" width="7" customWidth="1"/>
+    <col min="21" max="21" width="18" customWidth="1"/>
+    <col min="27" max="27" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
@@ -855,6 +875,9 @@
       <c r="L1" s="16" t="s">
         <v>13</v>
       </c>
+      <c r="N1" t="s">
+        <v>33</v>
+      </c>
       <c r="S1" s="13"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
@@ -1452,7 +1475,7 @@
       </c>
       <c r="S16" s="13"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>3</v>
       </c>
@@ -1508,7 +1531,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>4</v>
       </c>
@@ -1562,7 +1585,7 @@
       </c>
       <c r="S18" s="13"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>5</v>
       </c>
@@ -1601,7 +1624,7 @@
       </c>
       <c r="S19" s="13"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>6</v>
       </c>
@@ -1640,7 +1663,7 @@
       </c>
       <c r="S20" s="13"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>7</v>
       </c>
@@ -1683,28 +1706,36 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="13"/>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="V21" s="27"/>
+    </row>
+    <row r="22" spans="1:27" ht="15.6" x14ac:dyDescent="0.3">
       <c r="N22" s="2"/>
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="13"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="V22" s="27"/>
+      <c r="AA22" s="27"/>
+    </row>
+    <row r="23" spans="1:27" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N23" t="s">
+        <v>32</v>
+      </c>
       <c r="S23" s="13"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="AA23" s="27"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="N24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="S24" s="13"/>
-    </row>
-    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AA24" s="28"/>
+    </row>
+    <row r="25" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="S25" s="13"/>
     </row>
-    <row r="26" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N26" s="12" t="s">
         <v>2</v>
       </c>
@@ -1721,8 +1752,9 @@
         <v>21</v>
       </c>
       <c r="S26" s="13"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="AA26" s="13"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="N27" s="11">
         <v>0</v>
       </c>
@@ -1739,10 +1771,10 @@
         <v>1</v>
       </c>
       <c r="S27" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N28" s="9">
         <v>1</v>
       </c>
@@ -1758,23 +1790,20 @@
       <c r="R28" s="3">
         <v>1</v>
       </c>
-      <c r="S28" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="S29" s="13"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="N30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="S30" s="13"/>
     </row>
-    <row r="31" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="S31" s="13"/>
     </row>
-    <row r="32" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:27" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N32" s="12" t="s">
         <v>2</v>
       </c>
@@ -1809,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="S33" s="13" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="14:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1828,7 +1857,9 @@
       <c r="R34" s="3">
         <v>1</v>
       </c>
-      <c r="S34" s="13"/>
+      <c r="S34" s="29" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="35" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S35" s="13"/>
@@ -1838,7 +1869,7 @@
     </row>
     <row r="37" spans="14:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N37" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="S37" s="13"/>
     </row>
@@ -1877,7 +1908,7 @@
         <v>0</v>
       </c>
       <c r="S39" s="13" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="14:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -1896,7 +1927,7 @@
       <c r="R40" s="23">
         <v>0</v>
       </c>
-      <c r="S40" s="13"/>
+      <c r="S40" s="29"/>
     </row>
     <row r="41" spans="14:19" x14ac:dyDescent="0.3">
       <c r="S41" s="13"/>

</xml_diff>